<commit_message>
Dejo listo el bot para poder agregar credenciales de buzon
</commit_message>
<xml_diff>
--- a/Process/config/Config.xlsx
+++ b/Process/config/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laburo\VORTEX\PROYECTOS\01_RecupercionSoportes\Process\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laburo\VORTEX\PROYECTOS\01_RecuperacionSoportes\Process\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D0627E-5F2C-462D-8738-603D5831F924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F24EEA5-27E7-412D-98D0-A2576756C8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31020" yWindow="2196" windowWidth="18624" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="1776" windowWidth="18624" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Valor</t>
   </si>
@@ -129,9 +129,6 @@
     <t>CarpetaCompartida</t>
   </si>
   <si>
-    <t>C:/Users/lucas/Desktop/SharedFolderPrueba</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ruta carpeta compartida. </t>
   </si>
   <si>
@@ -139,9 +136,6 @@
   </si>
   <si>
     <t>Ruta al archivo insumo.</t>
-  </si>
-  <si>
-    <t>//10.238.99.5/temporales/ROCKETBOT/Copia de Inusmo busqueda masiva - UT Ticenergi.xlsx</t>
   </si>
   <si>
     <t>FALLO OBTENCION INSUMO</t>
@@ -179,6 +173,30 @@
   </si>
   <si>
     <t>URL de workmanager</t>
+  </si>
+  <si>
+    <t>O365</t>
+  </si>
+  <si>
+    <t>Credenciales O365</t>
+  </si>
+  <si>
+    <t>TenantId</t>
+  </si>
+  <si>
+    <t>024e2966-f777-426e-9ffb-80231972a6b1</t>
+  </si>
+  <si>
+    <t>Tenant ID de Azure</t>
+  </si>
+  <si>
+    <t>CredencialO365</t>
+  </si>
+  <si>
+    <t>//10.238.99.5/temporales/ROCKETBOT/Compartida</t>
+  </si>
+  <si>
+    <t>//10.238.99.5/temporales/ROCKETBOT/Inusmo busqueda masiva - UT Ticenergi.xlsx</t>
   </si>
 </sst>
 </file>
@@ -269,7 +287,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -303,6 +321,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -525,10 +546,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -615,32 +636,32 @@
         <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4">
         <v>500</v>
@@ -649,21 +670,49 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -710,7 +759,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>10</v>
@@ -724,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>22</v>
@@ -738,7 +787,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>11</v>
@@ -752,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>12</v>
@@ -760,16 +809,16 @@
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego cambios al config y una correccion de logica para las descargas de los archivos de WorkManager.
</commit_message>
<xml_diff>
--- a/Process/config/Config.xlsx
+++ b/Process/config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laburo\VORTEX\PROYECTOS\01_RecuperacionSoportes\Process\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F24EEA5-27E7-412D-98D0-A2576756C8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FE308E-2B12-4A80-A1C0-8936943B6B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1776" windowWidth="18624" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Valor</t>
   </si>
@@ -197,6 +197,16 @@
   </si>
   <si>
     <t>//10.238.99.5/temporales/ROCKETBOT/Inusmo busqueda masiva - UT Ticenergi.xlsx</t>
+  </si>
+  <si>
+    <t>FALLO LOGIN WORKMANAGER</t>
+  </si>
+  <si>
+    <t>[ERROR] | Fallo al realizar Login en workmanager | [NombreProceso] | [Fecha]</t>
+  </si>
+  <si>
+    <t>Estimados,
+Se ha producido un error al intentar iniciar sesión en WorkManager. Por favor, verificar si las credenciales de acceso han sido modificadas.</t>
   </si>
 </sst>
 </file>
@@ -548,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -722,22 +732,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFF535B-528C-3144-A844-11606A8F8BD2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="59" style="7" customWidth="1"/>
-    <col min="4" max="4" width="66" style="7" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -819,12 +829,27 @@
       </c>
       <c r="D6" s="8" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6D18D2D2-0A28-479C-A039-33D2F8A14053}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{FE32BF4A-8A8F-41DD-9F08-4D36175CB8F9}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{CA61B85D-0AAF-4D71-AF99-09A397CB6E30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modifico template de archivo de seguimiento. Actualizo scripts. Agrego logica para que se obtenga numero de proceso.
</commit_message>
<xml_diff>
--- a/Process/config/Config.xlsx
+++ b/Process/config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laburo\VORTEX\PROYECTOS\01_RecuperacionSoportes\Process\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FE308E-2B12-4A80-A1C0-8936943B6B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B55DD2-B251-4FB6-B5CA-440944FEDD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -558,8 +558,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="4">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>0</v>
@@ -734,7 +734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFF535B-528C-3144-A844-11606A8F8BD2}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se crea una copia de la bd en la carpeta backup dentro de bd, se impieza a unir la bd con las ultimas modificaciones de lucas en el navegador con lo realizado en siesa creando un bd en la que se empezara a funcionar la cual se nombra con v2
</commit_message>
<xml_diff>
--- a/Process/config/Config.xlsx
+++ b/Process/config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laburo\VORTEX\PROYECTOS\01_RecuperacionSoportes\Process\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B55DD2-B251-4FB6-B5CA-440944FEDD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EE9018-EBC1-4748-A5EC-B34A24311D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t>Valor</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>REPORTE</t>
-  </si>
-  <si>
-    <t>soporte@soporte.com</t>
   </si>
   <si>
     <t>Estimados, 
@@ -207,6 +204,42 @@
   <si>
     <t>Estimados,
 Se ha producido un error al intentar iniciar sesión en WorkManager. Por favor, verificar si las credenciales de acceso han sido modificadas.</t>
+  </si>
+  <si>
+    <t>contabilidad.finanzas@energizan,julian.lopez@energizando.com,yhonatan.ospina@energizando.com</t>
+  </si>
+  <si>
+    <t>FALLO AL VOLCAR INFORMACION DE SEGUIMIENTO</t>
+  </si>
+  <si>
+    <t>[ERROR] | Fallo al obtener datos a procesar | [NombreProceso] | [Fecha]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimados,
+Se ha producido un error al intentar obtener los datos necesarios para el procesamiento del flujo.
+</t>
+  </si>
+  <si>
+    <t>FALLO EN TRATAMIENTO DE ITEM</t>
+  </si>
+  <si>
+    <t>[ERROR] | Fallo al procesar el item [TipoDoc]-[NroDoc] | [NombreProceso] | [Fecha]</t>
+  </si>
+  <si>
+    <t>Estimados,
+Se ha producido un error al procesar el ítem [TipoDoc]-[NroDoc] dentro del flujo [NombreProceso].
+Por favor, verificar si el item presenta inconsistencias</t>
+  </si>
+  <si>
+    <t>FALLO EN ACTUALIZACION DE REPORTE</t>
+  </si>
+  <si>
+    <t>[ERROR] | Fallo en la actualizacion de reporte | [NombreProceso] | [Fecha]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimados,
+Se ha producido un error durante la actualización del reporte correspondiente al proceso [NombreProceso], ejecutado el día [Fecha].
+</t>
   </si>
 </sst>
 </file>
@@ -297,7 +330,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -320,9 +353,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -558,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -573,13 +603,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -587,91 +617,91 @@
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4">
         <v>200</v>
@@ -680,49 +710,49 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -732,32 +762,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFF535B-528C-3144-A844-11606A8F8BD2}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.21875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="62.77734375" style="7" customWidth="1"/>
     <col min="3" max="3" width="58.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="10.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -765,91 +795,135 @@
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
+      <c r="B4" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>9</v>
+      <c r="B5" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>9</v>
+        <v>33</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="8" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>56</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6D18D2D2-0A28-479C-A039-33D2F8A14053}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{FE32BF4A-8A8F-41DD-9F08-4D36175CB8F9}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{CA61B85D-0AAF-4D71-AF99-09A397CB6E30}"/>
+    <hyperlink ref="B3:B7" r:id="rId2" display="contabilidad.finanzas@energizan,julian.lopez@energizando.com,yhonatan.ospina@energizando.com" xr:uid="{BD4BB669-BAB4-4423-86D8-C91077543777}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{21B5FD5C-B912-4EA6-B912-1B5AA2BA47C3}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{ECA0DA68-3FE1-4FB2-8061-9DA04CD9A8AB}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{E39AC9FF-08A1-4F27-8620-9B2477E25E41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se realizo una modificacion en el bot 012_DescargarArchivosDeProceso donde se modifico el xpath para que busque una coincidencia directa con el id, para evitar errores de que aparescan varias coincidencias con el numero de id buscado ya que anteriormente se bucaba era con contiene el id
</commit_message>
<xml_diff>
--- a/Process/config/Config.xlsx
+++ b/Process/config/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laburo\VORTEX\PROYECTOS\01_RecuperacionSoportes\Process\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EE9018-EBC1-4748-A5EC-B34A24311D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C893198B-BEF1-4E42-91FE-0270B8C05BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>Valor</t>
   </si>
@@ -240,6 +240,12 @@
     <t xml:space="preserve">Estimados,
 Se ha producido un error durante la actualización del reporte correspondiente al proceso [NombreProceso], ejecutado el día [Fecha].
 </t>
+  </si>
+  <si>
+    <t>DiccionarioNavegacionSiesa</t>
+  </si>
+  <si>
+    <t>{'Financiero': 'f','Contabilidad General': 'g','Contab': 'n','Auditoria de Documentos': 'r','Consulta por Numero': 'n'}</t>
   </si>
 </sst>
 </file>
@@ -330,7 +336,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -365,6 +371,9 @@
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -586,16 +595,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="76.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="94.5546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="23" style="4" customWidth="1"/>
     <col min="4" max="4" width="118.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12.6640625" customWidth="1"/>
@@ -704,7 +713,7 @@
         <v>40</v>
       </c>
       <c r="B8" s="4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>0</v>
@@ -753,6 +762,14 @@
       </c>
       <c r="D11" s="4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFF535B-528C-3144-A844-11606A8F8BD2}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -777,7 +794,7 @@
     <col min="5" max="16384" width="10.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Version final con actualizacion - 06-11-2025
</commit_message>
<xml_diff>
--- a/Process/config/Config.xlsx
+++ b/Process/config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C893198B-BEF1-4E42-91FE-0270B8C05BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE09E9-B957-42F4-8A7F-DD85EEDAC344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
   <si>
     <t>Valor</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>{'Financiero': 'f','Contabilidad General': 'g','Contab': 'n','Auditoria de Documentos': 'r','Consulta por Numero': 'n'}</t>
+  </si>
+  <si>
+    <t>C:/Users/administrator.ENERGIZANDO/Desktop/SISTEMA UNO CLOUD.lnk</t>
+  </si>
+  <si>
+    <t>Diccionario para la nevagacion de Siesa</t>
+  </si>
+  <si>
+    <t>Link  a ejecutable de Siesa 8.5</t>
+  </si>
+  <si>
+    <t>RutaEjecutableSiesa</t>
   </si>
 </sst>
 </file>
@@ -595,10 +607,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="117" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -770,6 +782,26 @@
       </c>
       <c r="B12" s="13" t="s">
         <v>67</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>